<commit_message>
StateManager 0.7V + SkillRenewaling 1.4
</commit_message>
<xml_diff>
--- a/Assets/02Script/Manager/SkillManager/SkillSheet.xlsx
+++ b/Assets/02Script/Manager/SkillManager/SkillSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSK\Desktop\UnityGames\RPGGame\Assets\02Script\Manager\SkillManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF979172-3D2F-4F19-A69F-1B73393C0038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EC25D5-660A-460D-BC28-B36DEB01AB75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="4635" windowWidth="28800" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t>Index</t>
   </si>
@@ -35,39 +35,24 @@
     <t>Description</t>
   </si>
   <si>
-    <t>CanMove</t>
-  </si>
-  <si>
     <t>Single</t>
   </si>
   <si>
     <t>HitCount</t>
   </si>
   <si>
-    <t>During</t>
-  </si>
-  <si>
     <t>Multiple</t>
   </si>
   <si>
-    <t>Cooldown</t>
-  </si>
-  <si>
     <t>ParentIndex</t>
   </si>
   <si>
     <t>기본공격</t>
   </si>
   <si>
-    <t>non</t>
-  </si>
-  <si>
     <t>강타</t>
   </si>
   <si>
-    <t>전방의 다수의 적을 향해 강하게 타격한다.</t>
-  </si>
-  <si>
     <t>파이어볼</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -81,14 +66,6 @@
   </si>
   <si>
     <t>InfluencedBy</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DebuffIndex</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BuffIndex</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -200,10 +177,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>EndFrom</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Damage_Percentage</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -293,6 +266,209 @@
   </si>
   <si>
     <t>IsDetectCollision</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>가호</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>StateEffecterIndex</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>저주</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Curse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대상이 되는 적과 그 주변의 적에게 10초간 공격과 방어, 속도의 10%를 하락시킨다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>전방의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 적을 타격한다.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전방의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>적을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>향해</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강하게</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>타격한다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TargetTo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duration</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cooldown</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Friend</t>
+  </si>
+  <si>
+    <t>Friend</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoostMorale</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">자신 주변의 적들에게 피해를 주고, 자신은 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">초간 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>방어를 50% 상승시킨다.</t>
+    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -300,7 +476,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -310,6 +486,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -343,6 +520,41 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="돋움"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -364,12 +576,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -588,19 +802,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="35.85546875" customWidth="1"/>
-    <col min="5" max="7" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -608,140 +824,134 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="3">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1">
-        <v>0</v>
-      </c>
-      <c r="T2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="b">
+      <c r="D3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1">
         <v>50</v>
@@ -756,54 +966,51 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="3">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="3">
         <v>3</v>
       </c>
-      <c r="M3" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" t="b">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>56</v>
-      </c>
-      <c r="P3" s="1">
+      <c r="N3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="1">
         <v>5</v>
       </c>
-      <c r="Q3" s="1">
-        <v>1</v>
-      </c>
       <c r="R3" s="1">
         <v>1</v>
       </c>
       <c r="S3" s="1">
         <v>0</v>
       </c>
-      <c r="T3" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="b">
+        <v>10</v>
+      </c>
+      <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G4">
         <v>50</v>
@@ -818,54 +1025,51 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4">
         <v>5</v>
       </c>
-      <c r="M4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" t="b">
-        <v>1</v>
-      </c>
-      <c r="O4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4">
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4">
         <v>5</v>
       </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
       <c r="R4">
         <v>1</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
     </row>
-    <row r="5" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>4</v>
+    <row r="5" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1" t="b">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G5" s="3">
         <v>100</v>
@@ -880,25 +1084,25 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="3">
-        <v>5</v>
-      </c>
-      <c r="M5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O5" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="3">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="3">
         <v>10</v>
       </c>
+      <c r="N5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>18</v>
+      </c>
       <c r="Q5" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R5" s="3">
         <v>2</v>
@@ -906,28 +1110,25 @@
       <c r="S5" s="3">
         <v>0</v>
       </c>
-      <c r="T5" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>5</v>
+    <row r="6" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="1" t="b">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G6" s="3">
         <v>100</v>
@@ -942,25 +1143,25 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="3">
-        <v>5</v>
-      </c>
-      <c r="M6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O6" t="s">
-        <v>56</v>
-      </c>
-      <c r="P6" s="3">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="3">
         <v>10</v>
       </c>
+      <c r="N6" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>48</v>
+      </c>
       <c r="Q6" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="R6" s="3">
         <v>2</v>
@@ -968,24 +1169,133 @@
       <c r="S6" s="3">
         <v>0</v>
       </c>
-      <c r="T6" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+    <row r="7" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="3">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="3">
+        <v>10</v>
+      </c>
+      <c r="N7" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>15</v>
+      </c>
+      <c r="R7" s="3">
+        <v>2</v>
+      </c>
+      <c r="S7" s="3">
+        <v>4</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:20" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="3">
+        <v>10</v>
+      </c>
+      <c r="N8" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>15</v>
+      </c>
+      <c r="R8" s="1">
+        <v>2</v>
+      </c>
+      <c r="S8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="18" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -1017,25 +1327,25 @@
           <x14:formula1>
             <xm:f>시트2!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{DC176F6F-5325-449D-8619-7C5C70950DC9}">
-          <x14:formula1>
-            <xm:f>시트2!$C$2:$C$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>K2:K6</xm:sqref>
+          <xm:sqref>F2:F8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{42C580DA-13AA-4001-A5CC-E67AE20C1D0D}">
           <x14:formula1>
             <xm:f>시트2!$E$2:$E$5</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:N6</xm:sqref>
+          <xm:sqref>N2:O8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{300C056E-0D73-4768-8748-5335C4D6DCEB}">
           <x14:formula1>
             <xm:f>시트2!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O6</xm:sqref>
+          <xm:sqref>P2:P8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{DC176F6F-5325-449D-8619-7C5C70950DC9}">
+          <x14:formula1>
+            <xm:f>시트2!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:L8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1051,87 +1361,90 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stateEffecter + SkillManager Linked
</commit_message>
<xml_diff>
--- a/Assets/02Script/Manager/SkillManager/SkillSheet.xlsx
+++ b/Assets/02Script/Manager/SkillManager/SkillSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSK\Desktop\UnityGames\RPGGame\Assets\02Script\Manager\SkillManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EC25D5-660A-460D-BC28-B36DEB01AB75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC0632F-5026-4A89-B9B7-9ED619DFBC98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="4635" windowWidth="28800" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>Index</t>
   </si>
@@ -265,10 +265,6 @@
     <t>Ground</t>
   </si>
   <si>
-    <t>IsDetectCollision</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>가호</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -420,13 +416,24 @@
   </si>
   <si>
     <t>Friend</t>
-  </si>
-  <si>
-    <t>Friend</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>BoostMorale</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stamp</t>
+  </si>
+  <si>
+    <t>Stamp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monster</t>
+  </si>
+  <si>
+    <t>Monster</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -438,16 +445,7 @@
         <family val="2"/>
         <charset val="129"/>
       </rPr>
-      <t xml:space="preserve">자신 주변의 적들에게 피해를 주고, 자신은 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>10</t>
+      <t>자신</t>
     </r>
     <r>
       <rPr>
@@ -457,7 +455,26 @@
         <family val="2"/>
         <charset val="129"/>
       </rPr>
-      <t xml:space="preserve">초간 </t>
+      <t xml:space="preserve">은 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">초간 공격과 </t>
     </r>
     <r>
       <rPr>
@@ -802,10 +819,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -813,10 +830,10 @@
     <col min="4" max="4" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="18.85546875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -842,40 +859,37 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>44</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>60</v>
+      <c r="P1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -886,7 +900,7 @@
         <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -907,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="L2" t="s">
         <v>16</v>
@@ -916,25 +930,22 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" t="s">
         <v>18</v>
       </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
       <c r="Q2" s="1">
         <v>0</v>
       </c>
       <c r="R2" s="1">
         <v>0</v>
       </c>
-      <c r="S2" s="1">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -945,7 +956,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -966,7 +977,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
         <v>16</v>
@@ -975,25 +986,22 @@
         <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" t="s">
         <v>48</v>
       </c>
+      <c r="P3" s="1">
+        <v>5</v>
+      </c>
       <c r="Q3" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R3" s="1">
-        <v>1</v>
-      </c>
-      <c r="S3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1025,7 +1033,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="L4" t="s">
         <v>16</v>
@@ -1036,23 +1044,20 @@
       <c r="N4" t="s">
         <v>21</v>
       </c>
-      <c r="O4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="O4" t="s">
         <v>18</v>
       </c>
+      <c r="P4">
+        <v>5</v>
+      </c>
       <c r="Q4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>1</v>
-      </c>
-      <c r="S4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1084,7 +1089,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s">
         <v>18</v>
@@ -1093,25 +1098,22 @@
         <v>10</v>
       </c>
       <c r="N5" t="s">
-        <v>45</v>
-      </c>
-      <c r="O5" t="b">
-        <v>1</v>
-      </c>
-      <c r="P5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O5" t="s">
         <v>18</v>
       </c>
+      <c r="P5" s="3">
+        <v>10</v>
+      </c>
       <c r="Q5" s="3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="R5" s="3">
-        <v>2</v>
-      </c>
-      <c r="S5" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1137,51 +1139,48 @@
         <v>5</v>
       </c>
       <c r="I6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="L6" t="s">
         <v>16</v>
       </c>
       <c r="M6" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N6" t="s">
         <v>45</v>
       </c>
-      <c r="O6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="O6" t="s">
         <v>48</v>
       </c>
+      <c r="P6" s="3">
+        <v>10</v>
+      </c>
       <c r="Q6" s="3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="R6" s="3">
-        <v>2</v>
-      </c>
-      <c r="S6" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -1190,19 +1189,19 @@
         <v>29</v>
       </c>
       <c r="G7" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H7" s="3">
         <v>1</v>
       </c>
       <c r="I7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="L7" t="s">
         <v>16</v>
@@ -1211,36 +1210,33 @@
         <v>10</v>
       </c>
       <c r="N7" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7" t="s">
         <v>48</v>
       </c>
+      <c r="P7" s="3">
+        <v>15</v>
+      </c>
       <c r="Q7" s="3">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="R7" s="3">
-        <v>2</v>
-      </c>
-      <c r="S7" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -1255,13 +1251,13 @@
         <v>1</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="b">
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="L8" t="s">
         <v>18</v>
@@ -1270,32 +1266,29 @@
         <v>10</v>
       </c>
       <c r="N8" t="s">
-        <v>45</v>
-      </c>
-      <c r="O8" t="b">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" t="s">
         <v>48</v>
       </c>
+      <c r="P8" s="1">
+        <v>15</v>
+      </c>
       <c r="Q8" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="R8" s="1">
-        <v>2</v>
-      </c>
-      <c r="S8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:19" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:18" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:18" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:18" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:18" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:18" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:18" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:18" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:18" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="18" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -1329,23 +1322,23 @@
           </x14:formula1>
           <xm:sqref>F2:F8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{42C580DA-13AA-4001-A5CC-E67AE20C1D0D}">
-          <x14:formula1>
-            <xm:f>시트2!$E$2:$E$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>N2:O8</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{300C056E-0D73-4768-8748-5335C4D6DCEB}">
           <x14:formula1>
             <xm:f>시트2!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P8</xm:sqref>
+          <xm:sqref>O2:O8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{DC176F6F-5325-449D-8619-7C5C70950DC9}">
           <x14:formula1>
             <xm:f>시트2!$C$2:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>K2:L8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{4138A58B-0837-46A1-B592-F69EE22E07F2}">
+          <x14:formula1>
+            <xm:f>시트2!$E$2:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>N2:N8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1361,7 +1354,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1414,7 +1407,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>40</v>
@@ -1428,10 +1421,13 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>41</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="F4" s="2"/>
     </row>

</xml_diff>

<commit_message>
SkillRenewal 0.9, controllerRenewaling 0.5
</commit_message>
<xml_diff>
--- a/Assets/02Script/Manager/SkillManager/SkillSheet.xlsx
+++ b/Assets/02Script/Manager/SkillManager/SkillSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSK\Desktop\UnityGames\RPGGame\Assets\02Script\Manager\SkillManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SungyuJang\Desktop\GitHubDesktop\RPGGame\Assets\02Script\Manager\SkillManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC0632F-5026-4A89-B9B7-9ED619DFBC98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CCE699-4BC5-40C2-BD80-F2FE60E5F6BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -73,8 +73,329 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">전방에 </t>
+    <t>StartFrom</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character</t>
+  </si>
+  <si>
+    <t>Character</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>Enemy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Target</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>Line</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jump</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>어스퀘이크</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전방에 지진 물결을 일으킨다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Damage_Percentage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Physic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Physic</t>
+  </si>
+  <si>
+    <t>Magic</t>
+  </si>
+  <si>
+    <t>SkillTier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name_Eng</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NomalAttack</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LowSmash</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FireBall</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChaosBoom</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EarthQuake</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartRed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Straigth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wide</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forward</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Back</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllAround</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsSingleTarget</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jump</t>
+  </si>
+  <si>
+    <t>FXStartPoint</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ground</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>가호</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>StateEffecterIndex</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>저주</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Curse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대상이 되는 적과 그 주변의 적에게 10초간 공격과 방어, 속도의 10%를 하락시킨다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전방의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>적을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>향해</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강하게</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>타격한다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TargetTo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duration</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cooldown</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Friend</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoostMorale</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stamp</t>
+  </si>
+  <si>
+    <t>Stamp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monster</t>
+  </si>
+  <si>
+    <t>Monster</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>자신</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">은 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">초간 공격과 </t>
     </r>
     <r>
       <rPr>
@@ -84,7 +405,43 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>폭발하는</t>
+      <t>방어를 50% 상승시킨다.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전방의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 적을 타격한다.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전방에</t>
     </r>
     <r>
       <rPr>
@@ -103,7 +460,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>구체를</t>
+      <t>폭발하는</t>
     </r>
     <r>
       <rPr>
@@ -122,7 +479,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>떨어뜨린다</t>
+      <t>구체를</t>
     </r>
     <r>
       <rPr>
@@ -131,350 +488,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>.</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>StartFrom</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Character</t>
-  </si>
-  <si>
-    <t>Character</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enemy</t>
-  </si>
-  <si>
-    <t>Enemy</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Target</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Line</t>
-  </si>
-  <si>
-    <t>Line</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jump</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>어스퀘이크</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>전방에 지진 물결을 일으킨다</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Damage_Percentage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Physic</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Magic</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Physic</t>
-  </si>
-  <si>
-    <t>Magic</t>
-  </si>
-  <si>
-    <t>SkillTier</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name_Eng</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NomalAttack</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LowSmash</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FireBall</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ChaosBoom</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EarthQuake</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>StartRed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Straigth</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wide</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Forward</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Back</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AllAround</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IsSingleTarget</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jump</t>
-  </si>
-  <si>
-    <t>FXStartPoint</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ground</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ground</t>
-  </si>
-  <si>
-    <t>가호</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>StateEffecterIndex</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>저주</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Curse</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>대상이 되는 적과 그 주변의 적에게 10초간 공격과 방어, 속도의 10%를 하락시킨다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>전방의</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> 적을 타격한다.</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>전방의</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>적을</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>향해</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>강하게</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>타격한다</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TargetTo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Length</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Duration</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cooldown</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Friend</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoostMorale</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stamp</t>
-  </si>
-  <si>
-    <t>Stamp</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monster</t>
-  </si>
-  <si>
-    <t>Monster</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>자신</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">은 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">초간 공격과 </t>
     </r>
     <r>
       <rPr>
@@ -484,7 +498,16 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>방어를 50% 상승시킨다.</t>
+      <t>떨어뜨린다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -821,8 +844,8 @@
   </sheetPr>
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -841,7 +864,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -853,43 +876,43 @@
         <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -897,16 +920,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
@@ -921,19 +944,19 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M2" s="3">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
@@ -953,16 +976,16 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="1">
         <v>50</v>
@@ -977,19 +1000,19 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M3" s="3">
         <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P3" s="1">
         <v>5</v>
@@ -1009,7 +1032,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
@@ -1018,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4">
         <v>50</v>
@@ -1033,19 +1056,19 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M4">
         <v>5</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P4">
         <v>5</v>
@@ -1057,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1065,16 +1088,16 @@
         <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>35</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="3">
         <v>100</v>
@@ -1089,19 +1112,19 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M5" s="3">
         <v>10</v>
       </c>
       <c r="N5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P5" s="3">
         <v>10</v>
@@ -1118,19 +1141,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E6" s="3">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>100</v>
@@ -1145,19 +1168,19 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M6" s="3">
         <v>15</v>
       </c>
       <c r="N6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P6" s="3">
         <v>10</v>
@@ -1174,19 +1197,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -1201,19 +1224,19 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M7" s="3">
         <v>10</v>
       </c>
       <c r="N7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P7" s="3">
         <v>15</v>
@@ -1230,19 +1253,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -1257,19 +1280,19 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M8" s="3">
         <v>10</v>
       </c>
       <c r="N8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P8" s="1">
         <v>15</v>
@@ -1361,22 +1384,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1384,19 +1407,19 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1404,43 +1427,43 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>